<commit_message>
VAT of PS added in Bill
</commit_message>
<xml_diff>
--- a/ContractBillFormat.xlsx
+++ b/ContractBillFormat.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\VBStudio\CSAYContractManagementSoftware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE079142-E8FA-4911-A1E6-15AF98849E6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA311BF7-40C3-4C14-B4A4-5FE9BC6E761E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{193CE6FD-A91E-4DF5-B481-859DA899C5F3}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="43">
   <si>
     <t>Record 2023/06/26_20:51:22</t>
   </si>
@@ -140,6 +140,21 @@
   </si>
   <si>
     <t>Deduct Retention and taxes %</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>VAT Amount of PS</t>
+  </si>
+  <si>
+    <t>PS including VAT</t>
+  </si>
+  <si>
+    <t>Deduction% in VAT Amount</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -208,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -218,7 +233,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,7 +550,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,11 +630,11 @@
         <v>9</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="G6" s="1">
@@ -641,7 +655,7 @@
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G7" s="1">
@@ -666,7 +680,7 @@
       <c r="E8" s="4">
         <v>13</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="G8" s="1">
@@ -691,7 +705,7 @@
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="1" t="s">
         <v>16</v>
       </c>
       <c r="G9" s="1">
@@ -719,7 +733,7 @@
       <c r="E10" s="4">
         <v>0</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="G10" s="1">
@@ -746,7 +760,7 @@
       <c r="E11" s="4">
         <v>0</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G11" s="1">
@@ -773,7 +787,7 @@
       <c r="E12" s="4">
         <v>0</v>
       </c>
-      <c r="F12" s="7" t="s">
+      <c r="F12" s="1" t="s">
         <v>22</v>
       </c>
       <c r="G12" s="1">
@@ -796,7 +810,7 @@
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G13" s="1">
@@ -817,7 +831,7 @@
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="1" t="s">
         <v>26</v>
       </c>
       <c r="G14" s="1">
@@ -867,13 +881,16 @@
         <v>37</v>
       </c>
       <c r="G16" s="1">
-        <v>10.5</v>
+        <f>1.5+0.1+5</f>
+        <v>6.6</v>
       </c>
       <c r="H16" s="1">
-        <v>10.5</v>
+        <f t="shared" ref="H16:I16" si="0">1.5+0.1+5</f>
+        <v>6.6</v>
       </c>
       <c r="I16" s="1">
-        <v>10.5</v>
+        <f t="shared" si="0"/>
+        <v>6.6</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -896,6 +913,56 @@
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>12</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>13</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="1">
+        <v>30</v>
+      </c>
+      <c r="H19" s="1">
+        <v>30</v>
+      </c>
+      <c r="I19" s="1">
+        <v>30</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H21" t="s">

</xml_diff>